<commit_message>
test for input mtg / RSML
</commit_message>
<xml_diff>
--- a/test/inputs/Scenarios_24_06.xlsx
+++ b/test/inputs/Scenarios_24_06.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tigerault\package\Wheat-BRIDGES\Root_BRIDGES\root_cynaps\test\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AADCED27-F3B0-4812-8AC1-446B907A9FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B75EAD3-5416-4FF4-8335-1CD026890BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1708" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1744" uniqueCount="537">
   <si>
     <t>input_file</t>
   </si>
@@ -1639,6 +1639,12 @@
   </si>
   <si>
     <t>root_528.pckl</t>
+  </si>
+  <si>
+    <t>Input_RSML</t>
+  </si>
+  <si>
+    <t>M3591_47_LN_R4_D13.rsml</t>
   </si>
 </sst>
 </file>
@@ -2296,7 +2302,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2504,6 +2510,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2825,11 +2832,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H218"/>
+  <dimension ref="A1:I218"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
       <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H3" sqref="H3"/>
+      <selection pane="topRight" activeCell="E221" sqref="E221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2839,10 +2846,10 @@
     <col min="5" max="5" width="58.109375" customWidth="1"/>
     <col min="6" max="6" width="22.6640625" customWidth="1"/>
     <col min="7" max="7" width="19.5546875" style="37" customWidth="1"/>
-    <col min="8" max="8" width="39.88671875" style="1" customWidth="1"/>
+    <col min="8" max="9" width="39.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>468</v>
       </c>
@@ -2867,8 +2874,11 @@
       <c r="H1" s="36" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I1" s="36" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="74" t="s">
         <v>530</v>
       </c>
@@ -2893,8 +2903,11 @@
       <c r="H2" s="100" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="100" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>481</v>
       </c>
@@ -2919,8 +2932,11 @@
       <c r="H3" s="36" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I3" s="36" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>480</v>
       </c>
@@ -2945,8 +2961,11 @@
       <c r="H4" s="36" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I4" s="36" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>485</v>
       </c>
@@ -2971,8 +2990,11 @@
       <c r="H5" s="36" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I5" s="36" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>482</v>
       </c>
@@ -2997,8 +3019,11 @@
       <c r="H6" s="36" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" s="36" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
@@ -3023,8 +3048,11 @@
       <c r="H7" s="77" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" s="77" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
@@ -3049,8 +3077,11 @@
       <c r="H8" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="74" t="s">
         <v>443</v>
       </c>
@@ -3075,8 +3106,11 @@
       <c r="H9" s="77" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" s="77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>4</v>
       </c>
@@ -3101,8 +3135,11 @@
       <c r="H10" s="85">
         <v>180</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" s="85">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
@@ -3127,8 +3164,11 @@
       <c r="H11" s="78">
         <v>4.1666666999999998E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I11" s="78">
+        <v>4.1666666999999998E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>20</v>
       </c>
@@ -3153,8 +3193,11 @@
       <c r="H12" s="79">
         <v>4.1666666999999998E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12" s="79">
+        <v>4.1666666999999998E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>1</v>
       </c>
@@ -3179,8 +3222,11 @@
       <c r="H13" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I13" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>447</v>
       </c>
@@ -3205,8 +3251,11 @@
       <c r="H14" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>6</v>
       </c>
@@ -3231,8 +3280,11 @@
       <c r="H15" s="77" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I15" s="77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>7</v>
       </c>
@@ -3257,8 +3309,11 @@
       <c r="H16" s="80">
         <v>5.0000000000000001E-9</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16" s="80">
+        <v>5.0000000000000001E-9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>8</v>
       </c>
@@ -3283,8 +3338,11 @@
       <c r="H17" s="77">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I17" s="77">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>460</v>
       </c>
@@ -3309,8 +3367,11 @@
       <c r="H18" s="77" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I18" s="77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>461</v>
       </c>
@@ -3335,8 +3396,11 @@
       <c r="H19" s="77" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I19" s="77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>464</v>
       </c>
@@ -3361,8 +3425,11 @@
       <c r="H20" s="77" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I20" s="77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>466</v>
       </c>
@@ -3387,8 +3454,11 @@
       <c r="H21" s="77">
         <v>86400</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I21" s="77">
+        <v>86400</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>10</v>
       </c>
@@ -3413,8 +3483,11 @@
       <c r="H22" s="85" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I22" s="85" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>11</v>
       </c>
@@ -3439,8 +3512,11 @@
       <c r="H23" s="77">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I23" s="77">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>362</v>
       </c>
@@ -3465,8 +3541,11 @@
       <c r="H24" s="81" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I24" s="81" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>364</v>
       </c>
@@ -3491,8 +3570,11 @@
       <c r="H25" s="81" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I25" s="81" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>376</v>
       </c>
@@ -3517,8 +3599,11 @@
       <c r="H26" s="77" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I26" s="77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>375</v>
       </c>
@@ -3543,8 +3628,11 @@
       <c r="H27" s="81" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I27" s="81" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>374</v>
       </c>
@@ -3569,8 +3657,11 @@
       <c r="H28" s="81" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I28" s="81" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>12</v>
       </c>
@@ -3595,8 +3686,11 @@
       <c r="H29" s="77" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I29" s="77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>13</v>
       </c>
@@ -3621,8 +3715,11 @@
       <c r="H30" s="77">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I30" s="77">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
         <v>14</v>
       </c>
@@ -3647,8 +3744,11 @@
       <c r="H31" s="77" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I31" s="77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
         <v>9</v>
       </c>
@@ -3673,8 +3773,11 @@
       <c r="H32" s="77" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I32" s="77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
         <v>453</v>
       </c>
@@ -3699,8 +3802,11 @@
       <c r="H33" s="77" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I33" s="77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
         <v>21</v>
       </c>
@@ -3725,8 +3831,11 @@
       <c r="H34" s="77" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I34" s="77" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
         <v>22</v>
       </c>
@@ -3751,8 +3860,11 @@
       <c r="H35" s="85" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I35" s="85" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
         <v>23</v>
       </c>
@@ -3777,8 +3889,11 @@
       <c r="H36" s="80">
         <v>9.9999999999999995E-7</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I36" s="80">
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
         <v>24</v>
       </c>
@@ -3803,8 +3918,11 @@
       <c r="H37" s="86">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I37" s="86">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
         <v>25</v>
       </c>
@@ -3829,8 +3947,11 @@
       <c r="H38" s="77" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I38" s="77" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
         <v>26</v>
       </c>
@@ -3855,8 +3976,11 @@
       <c r="H39" s="77" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I39" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
         <v>27</v>
       </c>
@@ -3881,8 +4005,11 @@
       <c r="H40" s="77" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I40" s="77" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
         <v>28</v>
       </c>
@@ -3907,8 +4034,11 @@
       <c r="H41" s="77" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I41" s="77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
         <v>29</v>
       </c>
@@ -3933,8 +4063,11 @@
       <c r="H42" s="77">
         <v>120</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I42" s="77">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
         <v>30</v>
       </c>
@@ -3959,8 +4092,11 @@
       <c r="H43" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I43" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="13" t="s">
         <v>31</v>
       </c>
@@ -3985,8 +4121,11 @@
       <c r="H44" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I44" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>32</v>
       </c>
@@ -4011,8 +4150,11 @@
       <c r="H45" s="77">
         <v>-0.1</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I45" s="77">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="13" t="s">
         <v>33</v>
       </c>
@@ -4037,8 +4179,11 @@
       <c r="H46" s="77">
         <v>-0.2</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I46" s="77">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
         <v>34</v>
       </c>
@@ -4063,8 +4208,11 @@
       <c r="H47" s="77">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I47" s="77">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
         <v>35</v>
       </c>
@@ -4089,8 +4237,11 @@
       <c r="H48" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I48" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
         <v>433</v>
       </c>
@@ -4115,8 +4266,11 @@
       <c r="H49" s="77">
         <v>1200</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I49" s="77">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="13" t="s">
         <v>434</v>
       </c>
@@ -4141,8 +4295,11 @@
       <c r="H50" s="77">
         <v>1200</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I50" s="77">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
         <v>456</v>
       </c>
@@ -4167,8 +4324,11 @@
       <c r="H51" s="35" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I51" s="35" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="13" t="s">
         <v>15</v>
       </c>
@@ -4193,8 +4353,11 @@
       <c r="H52" s="77" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I52" s="77" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
         <v>16</v>
       </c>
@@ -4219,8 +4382,11 @@
       <c r="H53" s="77" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I53" s="77" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="11" t="s">
         <v>17</v>
       </c>
@@ -4245,8 +4411,11 @@
       <c r="H54" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I54" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="11" t="s">
         <v>18</v>
       </c>
@@ -4271,8 +4440,11 @@
       <c r="H55" s="77">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I55" s="77">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
         <v>19</v>
       </c>
@@ -4297,8 +4469,11 @@
       <c r="H56" s="77">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I56" s="77">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="15" t="s">
         <v>36</v>
       </c>
@@ -4323,8 +4498,11 @@
       <c r="H57" s="80">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I57" s="80">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="15" t="s">
         <v>379</v>
       </c>
@@ -4349,8 +4527,11 @@
       <c r="H58" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I58" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="15" t="s">
         <v>37</v>
       </c>
@@ -4375,8 +4556,11 @@
       <c r="H59" s="77">
         <v>1E-4</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I59" s="77">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="15" t="s">
         <v>38</v>
       </c>
@@ -4401,8 +4585,11 @@
       <c r="H60" s="77">
         <v>1E-4</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I60" s="77">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="17" t="s">
         <v>39</v>
       </c>
@@ -4427,8 +4614,11 @@
       <c r="H61" s="77">
         <v>6.9999999999999999E-4</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I61" s="77">
+        <v>6.9999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="17" t="s">
         <v>40</v>
       </c>
@@ -4453,8 +4643,11 @@
       <c r="H62" s="77">
         <v>1.22E-4</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I62" s="77">
+        <v>1.22E-4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="17" t="s">
         <v>206</v>
       </c>
@@ -4479,8 +4672,11 @@
       <c r="H63" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I63" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="17" t="s">
         <v>41</v>
       </c>
@@ -4505,8 +4701,11 @@
       <c r="H64" s="77">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I64" s="77">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="17" t="s">
         <v>405</v>
       </c>
@@ -4531,8 +4730,11 @@
       <c r="H65" s="77" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I65" s="77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="17" t="s">
         <v>90</v>
       </c>
@@ -4557,8 +4759,11 @@
       <c r="H66" s="77">
         <v>5</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I66" s="77">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="17" t="s">
         <v>407</v>
       </c>
@@ -4583,8 +4788,11 @@
       <c r="H67" s="77" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I67" s="77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="17" t="s">
         <v>42</v>
       </c>
@@ -4609,8 +4817,11 @@
       <c r="H68" s="77">
         <v>50</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I68" s="77">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="17" t="s">
         <v>207</v>
       </c>
@@ -4635,8 +4846,11 @@
       <c r="H69" s="78">
         <v>1453890.8941884842</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I69" s="78">
+        <v>1453890.8941884842</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="17" t="s">
         <v>43</v>
       </c>
@@ -4661,8 +4875,11 @@
       <c r="H70" s="78">
         <v>1.3888888888888888E-5</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I70" s="78">
+        <v>1.3888888888888888E-5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="17" t="s">
         <v>44</v>
       </c>
@@ -4687,8 +4904,11 @@
       <c r="H71" s="79">
         <v>6.5011574074074071E-4</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I71" s="79">
+        <v>6.5011574074074071E-4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="17" t="s">
         <v>45</v>
       </c>
@@ -4713,8 +4933,11 @@
       <c r="H72" s="85">
         <v>4.7400000000000003E-3</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I72" s="85">
+        <v>4.7400000000000003E-3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="17" t="s">
         <v>46</v>
       </c>
@@ -4739,8 +4962,11 @@
       <c r="H73" s="79">
         <v>282528</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I73" s="79">
+        <v>282528</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="17" t="s">
         <v>47</v>
       </c>
@@ -4765,8 +4991,11 @@
       <c r="H74" s="85">
         <v>0.56999999999999995</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I74" s="85">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="17" t="s">
         <v>48</v>
       </c>
@@ -4791,8 +5020,11 @@
       <c r="H75" s="87">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I75" s="87">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="17" t="s">
         <v>49</v>
       </c>
@@ -4817,8 +5049,11 @@
       <c r="H76" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I76" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="33" t="s">
         <v>50</v>
       </c>
@@ -4843,8 +5078,11 @@
       <c r="H77" s="78">
         <v>745476480000</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I77" s="78">
+        <v>745476480000</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="33" t="s">
         <v>204</v>
       </c>
@@ -4869,8 +5107,11 @@
       <c r="H78" s="77">
         <v>100</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I78" s="77">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="33" t="s">
         <v>413</v>
       </c>
@@ -4895,8 +5136,11 @@
       <c r="H79" s="77" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I79" s="77" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="33" t="s">
         <v>399</v>
       </c>
@@ -4921,8 +5165,11 @@
       <c r="H80" s="85">
         <v>21600</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I80" s="85">
+        <v>21600</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="33" t="s">
         <v>409</v>
       </c>
@@ -4947,8 +5194,11 @@
       <c r="H81" s="77">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I81" s="77">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="33" t="s">
         <v>400</v>
       </c>
@@ -4973,8 +5223,11 @@
       <c r="H82" s="85">
         <v>60479.999999999993</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I82" s="85">
+        <v>60479.999999999993</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="33" t="s">
         <v>410</v>
       </c>
@@ -4999,8 +5252,11 @@
       <c r="H83" s="77">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I83" s="77">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="33" t="s">
         <v>401</v>
       </c>
@@ -5025,8 +5281,11 @@
       <c r="H84" s="77">
         <v>518400</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I84" s="77">
+        <v>518400</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="33" t="s">
         <v>411</v>
       </c>
@@ -5051,8 +5310,11 @@
       <c r="H85" s="77">
         <v>5184000</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I85" s="77">
+        <v>5184000</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="17" t="s">
         <v>51</v>
       </c>
@@ -5077,8 +5339,11 @@
       <c r="H86" s="86">
         <v>50000</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I86" s="86">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="17" t="s">
         <v>52</v>
       </c>
@@ -5103,8 +5368,11 @@
       <c r="H87" s="77">
         <v>140000</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I87" s="77">
+        <v>140000</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="17" t="s">
         <v>53</v>
       </c>
@@ -5129,8 +5397,11 @@
       <c r="H88" s="78">
         <v>3.6636136999999999E-2</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I88" s="78">
+        <v>3.6636136999999999E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="17" t="s">
         <v>54</v>
       </c>
@@ -5155,8 +5426,11 @@
       <c r="H89" s="77">
         <v>4.4999999999999997E-3</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I89" s="77">
+        <v>4.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="17" t="s">
         <v>55</v>
       </c>
@@ -5181,8 +5455,11 @@
       <c r="H90" s="77">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I90" s="77">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="19" t="s">
         <v>213</v>
       </c>
@@ -5207,8 +5484,11 @@
       <c r="H91" s="77">
         <v>6.0000000000000002E-6</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I91" s="77">
+        <v>6.0000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="19" t="s">
         <v>214</v>
       </c>
@@ -5233,8 +5513,11 @@
       <c r="H92" s="77">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I92" s="77">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="19" t="s">
         <v>215</v>
       </c>
@@ -5259,8 +5542,11 @@
       <c r="H93" s="77">
         <v>374999999.99999994</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I93" s="77">
+        <v>374999999.99999994</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="19" t="s">
         <v>216</v>
       </c>
@@ -5285,8 +5571,11 @@
       <c r="H94" s="78">
         <v>3.7037037037037038E-3</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I94" s="78">
+        <v>3.7037037037037038E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="19" t="s">
         <v>217</v>
       </c>
@@ -5311,8 +5600,11 @@
       <c r="H95" s="77">
         <v>165600</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I95" s="77">
+        <v>165600</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="13" t="s">
         <v>60</v>
       </c>
@@ -5337,8 +5629,11 @@
       <c r="H96" s="77">
         <v>20</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I96" s="77">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="13" t="s">
         <v>208</v>
       </c>
@@ -5363,8 +5658,11 @@
       <c r="H97" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I97" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="13" t="s">
         <v>59</v>
       </c>
@@ -5389,8 +5687,11 @@
       <c r="H98" s="77">
         <v>21</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I98" s="77">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="23" t="s">
         <v>65</v>
       </c>
@@ -5415,8 +5716,11 @@
       <c r="H99" s="77">
         <v>0.64</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I99" s="77">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="23" t="s">
         <v>366</v>
       </c>
@@ -5441,8 +5745,11 @@
       <c r="H100" s="77">
         <v>8</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I100" s="77">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="23" t="s">
         <v>367</v>
       </c>
@@ -5467,8 +5774,11 @@
       <c r="H101" s="77">
         <v>10</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I101" s="77">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="23" t="s">
         <v>368</v>
       </c>
@@ -5493,8 +5803,11 @@
       <c r="H102" s="77">
         <v>8</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I102" s="77">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="23" t="s">
         <v>500</v>
       </c>
@@ -5519,8 +5832,11 @@
       <c r="H103" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I103" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="23" t="s">
         <v>384</v>
       </c>
@@ -5545,8 +5861,11 @@
       <c r="H104" s="77">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I104" s="77">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" s="23" t="s">
         <v>501</v>
       </c>
@@ -5573,8 +5892,12 @@
         <f>H103</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I105" s="58">
+        <f>I103</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="23" t="s">
         <v>502</v>
       </c>
@@ -5601,8 +5924,12 @@
         <f>150*H103</f>
         <v>150</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I106" s="58">
+        <f>150*I103</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" s="23" t="s">
         <v>503</v>
       </c>
@@ -5629,8 +5956,12 @@
         <f>H98</f>
         <v>21</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I107" s="58">
+        <f>I98</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" s="23" t="s">
         <v>504</v>
       </c>
@@ -5657,8 +5988,12 @@
         <f>70*H98</f>
         <v>1470</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I108" s="58">
+        <f>70*I98</f>
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" s="23" t="s">
         <v>386</v>
       </c>
@@ -5683,8 +6018,11 @@
       <c r="H109" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I109" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" s="23" t="s">
         <v>388</v>
       </c>
@@ -5709,8 +6047,11 @@
       <c r="H110" s="82">
         <v>1589759.9999999998</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I110" s="82">
+        <v>1589759.9999999998</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" s="23" t="s">
         <v>390</v>
       </c>
@@ -5735,8 +6076,11 @@
       <c r="H111" s="82">
         <v>6171428.5714285718</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I111" s="82">
+        <v>6171428.5714285718</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" s="23" t="s">
         <v>392</v>
       </c>
@@ -5761,8 +6105,11 @@
       <c r="H112" s="82">
         <v>6171428.5714285718</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I112" s="82">
+        <v>6171428.5714285718</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" s="23" t="s">
         <v>420</v>
       </c>
@@ -5787,8 +6134,11 @@
       <c r="H113" s="82">
         <v>100</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I113" s="82">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="23" t="s">
         <v>422</v>
       </c>
@@ -5815,8 +6165,12 @@
         <f>0.1 * 3.25 * (60*60*24)</f>
         <v>28080</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I114" s="67">
+        <f>0.1 * 3.25 * (60*60*24)</f>
+        <v>28080</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" s="23" t="s">
         <v>424</v>
       </c>
@@ -5843,8 +6197,12 @@
         <f>1.11 / 10</f>
         <v>0.11100000000000002</v>
       </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I115" s="67">
+        <f>1.11 / 10</f>
+        <v>0.11100000000000002</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" s="23" t="s">
         <v>497</v>
       </c>
@@ -5869,8 +6227,11 @@
       <c r="H116" s="82">
         <v>100</v>
       </c>
-    </row>
-    <row r="117" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I116" s="82">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="23" t="s">
         <v>498</v>
       </c>
@@ -5897,8 +6258,12 @@
         <f>5.32 * (60*60*24)</f>
         <v>459648</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I117" s="67">
+        <f>5.32 * (60*60*24)</f>
+        <v>459648</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" s="23" t="s">
         <v>499</v>
       </c>
@@ -5925,8 +6290,12 @@
         <f>1.11/8</f>
         <v>0.13875000000000001</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I118" s="67">
+        <f>1.11/8</f>
+        <v>0.13875000000000001</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" s="23" t="s">
         <v>394</v>
       </c>
@@ -5951,8 +6320,11 @@
       <c r="H119" s="82">
         <v>21600</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I119" s="82">
+        <v>21600</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" s="23" t="s">
         <v>396</v>
       </c>
@@ -5977,8 +6349,11 @@
       <c r="H120" s="88">
         <v>43200</v>
       </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I120" s="88">
+        <v>43200</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" s="13" t="s">
         <v>61</v>
       </c>
@@ -6003,8 +6378,11 @@
       <c r="H121" s="77">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I121" s="77">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" s="13" t="s">
         <v>62</v>
       </c>
@@ -6030,8 +6408,12 @@
         <f>1250*0.000001/6</f>
         <v>2.0833333333333335E-4</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I122" s="78">
+        <f>1250*0.000001/6</f>
+        <v>2.0833333333333335E-4</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" s="13" t="s">
         <v>63</v>
       </c>
@@ -6056,8 +6438,11 @@
       <c r="H123" s="77">
         <v>5.7899999999999998E-7</v>
       </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I123" s="77">
+        <v>5.7899999999999998E-7</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" s="13" t="s">
         <v>64</v>
       </c>
@@ -6082,8 +6467,11 @@
       <c r="H124" s="78">
         <v>2.0833333333333335E-4</v>
       </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I124" s="78">
+        <v>2.0833333333333335E-4</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" s="13" t="s">
         <v>449</v>
       </c>
@@ -6108,8 +6496,11 @@
       <c r="H125" s="78">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I125" s="78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" s="13" t="s">
         <v>451</v>
       </c>
@@ -6134,8 +6525,11 @@
       <c r="H126" s="78">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I126" s="78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="68" t="s">
         <v>440</v>
       </c>
@@ -6158,8 +6552,11 @@
       <c r="H127" s="89">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I127" s="89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" s="68" t="s">
         <v>67</v>
       </c>
@@ -6182,8 +6579,11 @@
       <c r="H128" s="89">
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I128" s="89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" s="68" t="s">
         <v>445</v>
       </c>
@@ -6208,8 +6608,11 @@
       <c r="H129" s="89" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I129" s="89" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" s="21" t="s">
         <v>66</v>
       </c>
@@ -6234,8 +6637,11 @@
       <c r="H130" s="83">
         <v>5.0000000000000001E-4</v>
       </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I130" s="83">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" s="21" t="s">
         <v>437</v>
       </c>
@@ -6260,8 +6666,11 @@
       <c r="H131" s="83">
         <v>4.9999999999999999E-13</v>
       </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I131" s="83">
+        <v>4.9999999999999999E-13</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" s="21" t="s">
         <v>228</v>
       </c>
@@ -6286,8 +6695,11 @@
       <c r="H132" s="77">
         <v>10</v>
       </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I132" s="77">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" s="21" t="s">
         <v>229</v>
       </c>
@@ -6312,8 +6724,11 @@
       <c r="H133" s="77">
         <v>-0.04</v>
       </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I133" s="77">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" s="21" t="s">
         <v>230</v>
       </c>
@@ -6338,8 +6753,11 @@
       <c r="H134" s="77">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I134" s="77">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" s="21" t="s">
         <v>231</v>
       </c>
@@ -6364,8 +6782,11 @@
       <c r="H135" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I135" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" s="21" t="s">
         <v>68</v>
       </c>
@@ -6390,8 +6811,11 @@
       <c r="H136" s="80">
         <v>1.9999999999999999E-7</v>
       </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I136" s="80">
+        <v>1.9999999999999999E-7</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" s="21" t="s">
         <v>232</v>
       </c>
@@ -6416,8 +6840,11 @@
       <c r="H137" s="77">
         <v>10</v>
       </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I137" s="77">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" s="21" t="s">
         <v>233</v>
       </c>
@@ -6442,8 +6869,11 @@
       <c r="H138" s="77">
         <v>-0.04</v>
       </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I138" s="77">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" s="21" t="s">
         <v>234</v>
       </c>
@@ -6468,8 +6898,11 @@
       <c r="H139" s="77">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I139" s="77">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" s="21" t="s">
         <v>235</v>
       </c>
@@ -6494,8 +6927,11 @@
       <c r="H140" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I140" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" s="21" t="s">
         <v>69</v>
       </c>
@@ -6520,8 +6956,11 @@
       <c r="H141" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I141" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142" s="72" t="s">
         <v>70</v>
       </c>
@@ -6546,8 +6985,11 @@
       <c r="H142" s="80">
         <v>5.0000000000000004E-6</v>
       </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I142" s="80">
+        <v>5.0000000000000004E-6</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" s="23" t="s">
         <v>56</v>
       </c>
@@ -6572,8 +7014,11 @@
       <c r="H143" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I143" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" s="23" t="s">
         <v>57</v>
       </c>
@@ -6598,8 +7043,11 @@
       <c r="H144" s="77">
         <v>2E-3</v>
       </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I144" s="77">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" s="23" t="s">
         <v>58</v>
       </c>
@@ -6624,8 +7072,11 @@
       <c r="H145" s="80">
         <v>3.9999999999999998E-6</v>
       </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I145" s="80">
+        <v>3.9999999999999998E-6</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146" s="23" t="s">
         <v>71</v>
       </c>
@@ -6650,8 +7101,11 @@
       <c r="H146" s="80">
         <v>3.7699999999999999E-10</v>
       </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I146" s="80">
+        <v>3.7699999999999999E-10</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147" s="23" t="s">
         <v>236</v>
       </c>
@@ -6676,8 +7130,11 @@
       <c r="H147" s="77">
         <v>20</v>
       </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I147" s="77">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148" s="23" t="s">
         <v>237</v>
       </c>
@@ -6702,8 +7159,11 @@
       <c r="H148" s="77">
         <v>-0.06</v>
       </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I148" s="77">
+        <v>-0.06</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149" s="23" t="s">
         <v>238</v>
       </c>
@@ -6728,8 +7188,11 @@
       <c r="H149" s="77">
         <v>0.89100000000000001</v>
       </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I149" s="77">
+        <v>0.89100000000000001</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150" s="23" t="s">
         <v>239</v>
       </c>
@@ -6754,8 +7217,11 @@
       <c r="H150" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I150" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" s="23" t="s">
         <v>72</v>
       </c>
@@ -6780,8 +7246,11 @@
       <c r="H151" s="80">
         <v>4.0000000000000003E-5</v>
       </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I151" s="80">
+        <v>4.0000000000000003E-5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152" s="13" t="s">
         <v>73</v>
       </c>
@@ -6806,8 +7275,11 @@
       <c r="H152" s="80">
         <v>5.8333333333333335E-9</v>
       </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I152" s="80">
+        <v>5.8333333333333335E-9</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153" s="13" t="s">
         <v>240</v>
       </c>
@@ -6832,8 +7304,11 @@
       <c r="H153" s="77">
         <v>20</v>
       </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I153" s="77">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154" s="13" t="s">
         <v>241</v>
       </c>
@@ -6858,8 +7333,11 @@
       <c r="H154" s="77">
         <v>-0.06</v>
       </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I154" s="77">
+        <v>-0.06</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A155" s="13" t="s">
         <v>242</v>
       </c>
@@ -6884,8 +7362,11 @@
       <c r="H155" s="77">
         <v>0.89100000000000001</v>
       </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I155" s="77">
+        <v>0.89100000000000001</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" s="13" t="s">
         <v>243</v>
       </c>
@@ -6910,8 +7391,11 @@
       <c r="H156" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I156" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157" s="13" t="s">
         <v>74</v>
       </c>
@@ -6936,8 +7420,11 @@
       <c r="H157" s="80">
         <v>4.0000000000000003E-5</v>
       </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I157" s="80">
+        <v>4.0000000000000003E-5</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158" s="9" t="s">
         <v>75</v>
       </c>
@@ -6962,8 +7449,11 @@
       <c r="H158" s="83">
         <v>4.0000000000000001E-8</v>
       </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I158" s="83">
+        <v>4.0000000000000001E-8</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159" s="9" t="s">
         <v>218</v>
       </c>
@@ -6988,8 +7478,11 @@
       <c r="H159" s="77">
         <v>20</v>
       </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I159" s="77">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A160" s="9" t="s">
         <v>219</v>
       </c>
@@ -7014,8 +7507,11 @@
       <c r="H160" s="77">
         <v>-4.4200000000000003E-2</v>
       </c>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I160" s="77">
+        <v>-4.4200000000000003E-2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A161" s="9" t="s">
         <v>220</v>
       </c>
@@ -7040,8 +7536,11 @@
       <c r="H161" s="77">
         <v>1.55</v>
       </c>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I161" s="77">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A162" s="9" t="s">
         <v>221</v>
       </c>
@@ -7066,8 +7565,11 @@
       <c r="H162" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I162" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A163" s="9" t="s">
         <v>76</v>
       </c>
@@ -7092,8 +7594,11 @@
       <c r="H163" s="77">
         <v>2.7799999999999998E-4</v>
       </c>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I163" s="77">
+        <v>2.7799999999999998E-4</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A164" s="25" t="s">
         <v>78</v>
       </c>
@@ -7118,8 +7623,11 @@
       <c r="H164" s="84">
         <v>2.4999999999999998E-12</v>
       </c>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I164" s="84">
+        <v>2.4999999999999998E-12</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A165" s="25" t="s">
         <v>245</v>
       </c>
@@ -7144,8 +7652,11 @@
       <c r="H165" s="77">
         <v>20</v>
       </c>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I165" s="77">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A166" s="25" t="s">
         <v>246</v>
       </c>
@@ -7170,8 +7681,11 @@
       <c r="H166" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I166" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A167" s="25" t="s">
         <v>247</v>
       </c>
@@ -7196,8 +7710,11 @@
       <c r="H167" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I167" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A168" s="25" t="s">
         <v>248</v>
       </c>
@@ -7222,8 +7739,11 @@
       <c r="H168" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I168" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A169" s="25" t="s">
         <v>79</v>
       </c>
@@ -7248,8 +7768,11 @@
       <c r="H169" s="77">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I169" s="77">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A170" s="31" t="s">
         <v>80</v>
       </c>
@@ -7274,8 +7797,11 @@
       <c r="H170" s="86">
         <v>2.0000000000000001E-9</v>
       </c>
-    </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I170" s="86">
+        <v>2.0000000000000001E-9</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A171" s="31" t="s">
         <v>249</v>
       </c>
@@ -7300,8 +7826,11 @@
       <c r="H171" s="77">
         <v>25</v>
       </c>
-    </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I171" s="77">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A172" s="31" t="s">
         <v>250</v>
       </c>
@@ -7326,8 +7855,11 @@
       <c r="H172" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I172" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A173" s="31" t="s">
         <v>251</v>
       </c>
@@ -7352,8 +7884,11 @@
       <c r="H173" s="77">
         <v>3.98</v>
       </c>
-    </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I173" s="77">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A174" s="31" t="s">
         <v>252</v>
       </c>
@@ -7378,8 +7913,11 @@
       <c r="H174" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I174" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A175" s="31" t="s">
         <v>81</v>
       </c>
@@ -7404,8 +7942,11 @@
       <c r="H175" s="78">
         <v>1.6666666666666666E-4</v>
       </c>
-    </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I175" s="78">
+        <v>1.6666666666666666E-4</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A176" s="11" t="s">
         <v>253</v>
       </c>
@@ -7430,8 +7971,11 @@
       <c r="H176" s="80">
         <v>1E-8</v>
       </c>
-    </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I176" s="80">
+        <v>1E-8</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A177" s="11" t="s">
         <v>254</v>
       </c>
@@ -7456,8 +8000,11 @@
       <c r="H177" s="77">
         <v>20</v>
       </c>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I177" s="77">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A178" s="11" t="s">
         <v>255</v>
       </c>
@@ -7482,8 +8029,11 @@
       <c r="H178" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I178" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A179" s="11" t="s">
         <v>256</v>
       </c>
@@ -7508,8 +8058,11 @@
       <c r="H179" s="77">
         <v>2</v>
       </c>
-    </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I179" s="77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A180" s="11" t="s">
         <v>257</v>
       </c>
@@ -7534,8 +8087,11 @@
       <c r="H180" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I180" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A181" s="11" t="s">
         <v>258</v>
       </c>
@@ -7560,8 +8116,11 @@
       <c r="H181" s="78">
         <v>8.3333333333333331E-5</v>
       </c>
-    </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I181" s="78">
+        <v>8.3333333333333331E-5</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A182" s="11" t="s">
         <v>259</v>
       </c>
@@ -7586,8 +8145,11 @@
       <c r="H182" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I182" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A183" s="27" t="s">
         <v>260</v>
       </c>
@@ -7612,8 +8174,11 @@
       <c r="H183" s="77">
         <v>2.3533050791148899E-8</v>
       </c>
-    </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I183" s="77">
+        <v>2.3533050791148899E-8</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A184" s="27" t="s">
         <v>261</v>
       </c>
@@ -7638,8 +8203,11 @@
       <c r="H184" s="77">
         <v>20</v>
       </c>
-    </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I184" s="77">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A185" s="27" t="s">
         <v>262</v>
       </c>
@@ -7664,8 +8232,11 @@
       <c r="H185" s="77">
         <v>-0.187</v>
       </c>
-    </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I185" s="77">
+        <v>-0.187</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A186" s="27" t="s">
         <v>263</v>
       </c>
@@ -7690,8 +8261,11 @@
       <c r="H186" s="77">
         <v>2.48</v>
       </c>
-    </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I186" s="77">
+        <v>2.48</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A187" s="27" t="s">
         <v>264</v>
       </c>
@@ -7716,8 +8290,11 @@
       <c r="H187" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I187" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A188" s="27" t="s">
         <v>265</v>
       </c>
@@ -7742,8 +8319,11 @@
       <c r="H188" s="77">
         <v>6.1060227588121015E-4</v>
       </c>
-    </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I188" s="77">
+        <v>6.1060227588121015E-4</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A189" s="23" t="s">
         <v>266</v>
       </c>
@@ -7768,8 +8348,11 @@
       <c r="H189" s="85">
         <v>3.9999999999999998E-7</v>
       </c>
-    </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I189" s="85">
+        <v>3.9999999999999998E-7</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A190" s="23" t="s">
         <v>267</v>
       </c>
@@ -7794,8 +8377,11 @@
       <c r="H190" s="77">
         <v>25</v>
       </c>
-    </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I190" s="77">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A191" s="23" t="s">
         <v>268</v>
       </c>
@@ -7820,8 +8406,11 @@
       <c r="H191" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I191" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A192" s="23" t="s">
         <v>269</v>
       </c>
@@ -7846,8 +8435,11 @@
       <c r="H192" s="77">
         <v>3.98</v>
       </c>
-    </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I192" s="77">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A193" s="23" t="s">
         <v>270</v>
       </c>
@@ -7872,8 +8464,11 @@
       <c r="H193" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I193" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A194" s="23" t="s">
         <v>271</v>
       </c>
@@ -7898,8 +8493,11 @@
       <c r="H194" s="78">
         <v>8.3333333333333331E-5</v>
       </c>
-    </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I194" s="78">
+        <v>8.3333333333333331E-5</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A195" s="7" t="s">
         <v>272</v>
       </c>
@@ -7924,8 +8522,11 @@
       <c r="H195" s="85">
         <v>3.9999999999999998E-7</v>
       </c>
-    </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I195" s="85">
+        <v>3.9999999999999998E-7</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A196" s="7" t="s">
         <v>273</v>
       </c>
@@ -7950,8 +8551,11 @@
       <c r="H196" s="77">
         <v>25</v>
       </c>
-    </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I196" s="77">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A197" s="7" t="s">
         <v>274</v>
       </c>
@@ -7976,8 +8580,11 @@
       <c r="H197" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I197" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A198" s="7" t="s">
         <v>275</v>
       </c>
@@ -8002,8 +8609,11 @@
       <c r="H198" s="77">
         <v>3.98</v>
       </c>
-    </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I198" s="77">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A199" s="7" t="s">
         <v>276</v>
       </c>
@@ -8028,8 +8638,11 @@
       <c r="H199" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I199" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A200" s="7" t="s">
         <v>277</v>
       </c>
@@ -8054,8 +8667,11 @@
       <c r="H200" s="78">
         <v>8.3333333333333331E-5</v>
       </c>
-    </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I200" s="78">
+        <v>8.3333333333333331E-5</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A201" s="29" t="s">
         <v>278</v>
       </c>
@@ -8080,8 +8696,11 @@
       <c r="H201" s="85">
         <v>1.9999999999999999E-7</v>
       </c>
-    </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I201" s="85">
+        <v>1.9999999999999999E-7</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A202" s="29" t="s">
         <v>279</v>
       </c>
@@ -8106,8 +8725,11 @@
       <c r="H202" s="77">
         <v>25</v>
       </c>
-    </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I202" s="77">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A203" s="29" t="s">
         <v>280</v>
       </c>
@@ -8132,8 +8754,11 @@
       <c r="H203" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I203" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A204" s="29" t="s">
         <v>281</v>
       </c>
@@ -8158,8 +8783,11 @@
       <c r="H204" s="77">
         <v>3.98</v>
       </c>
-    </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I204" s="77">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A205" s="29" t="s">
         <v>282</v>
       </c>
@@ -8184,8 +8812,11 @@
       <c r="H205" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I205" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A206" s="29" t="s">
         <v>283</v>
       </c>
@@ -8210,15 +8841,18 @@
       <c r="H206" s="78">
         <v>8.3333333333333331E-5</v>
       </c>
-    </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I206" s="78">
+        <v>8.3333333333333331E-5</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A207" s="90" t="s">
         <v>361</v>
       </c>
       <c r="B207" s="91" t="s">
         <v>470</v>
       </c>
-      <c r="C207" s="2" t="s">
+      <c r="C207" s="92" t="s">
         <v>529</v>
       </c>
       <c r="D207" s="92" t="s">
@@ -8236,8 +8870,11 @@
       <c r="H207" s="95" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="208" spans="1:8" s="96" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I207" s="95" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" s="101" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A208" s="2" t="s">
         <v>490</v>
       </c>
@@ -8262,8 +8899,11 @@
       <c r="H208" s="2">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="209" spans="1:8" s="96" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I208" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" s="101" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A209" s="2" t="s">
         <v>494</v>
       </c>
@@ -8288,8 +8928,11 @@
       <c r="H209" s="98">
         <v>-100000</v>
       </c>
-    </row>
-    <row r="210" spans="1:8" s="96" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I209" s="98">
+        <v>-100000</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" s="101" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A210" s="2" t="s">
         <v>516</v>
       </c>
@@ -8315,8 +8958,12 @@
         <f>H209</f>
         <v>-100000</v>
       </c>
-    </row>
-    <row r="211" spans="1:8" s="96" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I210" s="98">
+        <f>I209</f>
+        <v>-100000</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" s="101" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A211" s="2" t="s">
         <v>507</v>
       </c>
@@ -8341,8 +8988,11 @@
       <c r="H211" s="99">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="212" spans="1:8" s="96" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I211" s="99">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" s="101" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
         <v>508</v>
       </c>
@@ -8367,8 +9017,11 @@
       <c r="H212" s="99" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="213" spans="1:8" s="96" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I212" s="99" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" s="101" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A213" s="2" t="s">
         <v>509</v>
       </c>
@@ -8393,8 +9046,11 @@
       <c r="H213" s="99">
         <v>0</v>
       </c>
-    </row>
-    <row r="214" spans="1:8" s="96" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I213" s="99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" s="101" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A214" s="2" t="s">
         <v>510</v>
       </c>
@@ -8419,8 +9075,11 @@
       <c r="H214" s="99">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I214" s="99">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A215" s="2" t="s">
         <v>518</v>
       </c>
@@ -8445,8 +9104,11 @@
       <c r="H215" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I215" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A216" s="2" t="s">
         <v>520</v>
       </c>
@@ -8473,8 +9135,12 @@
         <f>1250*0.000001/5</f>
         <v>2.5000000000000001E-4</v>
       </c>
-    </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I216" s="98">
+        <f>1250*0.000001/5</f>
+        <v>2.5000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A217" s="2" t="s">
         <v>523</v>
       </c>
@@ -8499,8 +9165,11 @@
       <c r="H217" s="99">
         <v>9.9999999999999994E-12</v>
       </c>
-    </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I217" s="99">
+        <v>9.9999999999999994E-12</v>
+      </c>
+    </row>
+    <row r="218" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A218" s="2" t="s">
         <v>526</v>
       </c>
@@ -8525,9 +9194,12 @@
       <c r="H218" s="98">
         <v>2.0000000000000001E-4</v>
       </c>
+      <c r="I218" s="98">
+        <v>2.0000000000000001E-4</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H125:H126">
+  <conditionalFormatting sqref="H125:I126">
     <cfRule type="colorScale" priority="243">
       <colorScale>
         <cfvo type="min"/>
@@ -8539,7 +9211,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H130">
+  <conditionalFormatting sqref="H130:I130">
     <cfRule type="colorScale" priority="244">
       <colorScale>
         <cfvo type="min"/>
@@ -8561,7 +9233,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H131">
+  <conditionalFormatting sqref="H131:I131">
     <cfRule type="colorScale" priority="246">
       <colorScale>
         <cfvo type="min"/>
@@ -8583,7 +9255,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H136">
+  <conditionalFormatting sqref="H136:I136">
     <cfRule type="colorScale" priority="248">
       <colorScale>
         <cfvo type="min"/>
@@ -8595,7 +9267,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H142">
+  <conditionalFormatting sqref="H142:I142">
     <cfRule type="colorScale" priority="249">
       <colorScale>
         <cfvo type="min"/>
@@ -8627,7 +9299,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H158">
+  <conditionalFormatting sqref="H158:I158">
     <cfRule type="colorScale" priority="252">
       <colorScale>
         <cfvo type="min"/>
@@ -8659,7 +9331,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H164">
+  <conditionalFormatting sqref="H164:I164">
     <cfRule type="colorScale" priority="255">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>